<commit_message>
Add quarterly predictions data in Excel format for analysis
</commit_message>
<xml_diff>
--- a/data/others/annual_predictions_amd_fcx_ea.xlsx
+++ b/data/others/annual_predictions_amd_fcx_ea.xlsx
@@ -506,7 +506,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -549,7 +549,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E3" t="n">
@@ -592,7 +592,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E21" t="n">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E22" t="n">
@@ -1409,7 +1409,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E23" t="n">
@@ -1452,7 +1452,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E24" t="n">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E25" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E26" t="n">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -1624,7 +1624,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E28" t="n">
@@ -1667,7 +1667,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E29" t="n">
@@ -1710,7 +1710,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E33" t="n">
@@ -1882,7 +1882,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -1968,7 +1968,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E36" t="n">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E37" t="n">
@@ -2054,7 +2054,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E38" t="n">
@@ -2097,7 +2097,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E39" t="n">
@@ -2140,7 +2140,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E40" t="n">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -2224,7 +2224,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E43" t="n">
@@ -2310,7 +2310,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E44" t="n">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E45" t="n">
@@ -2396,7 +2396,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E46" t="n">
@@ -2439,7 +2439,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E47" t="n">
@@ -2482,7 +2482,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E48" t="n">
@@ -2525,7 +2525,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E49" t="n">
@@ -2568,7 +2568,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E50" t="n">
@@ -2611,7 +2611,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E51" t="n">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E52" t="n">
@@ -2697,7 +2697,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E53" t="n">
@@ -2740,7 +2740,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E54" t="n">
@@ -2783,7 +2783,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Materials</t>
+          <t>Basic Materials</t>
         </is>
       </c>
       <c r="E55" t="n">
@@ -4147,7 +4147,7 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E87" t="n">
@@ -4190,7 +4190,7 @@
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E88" t="n">
@@ -4233,7 +4233,7 @@
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E89" t="n">
@@ -4276,7 +4276,7 @@
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E90" t="n">
@@ -4319,7 +4319,7 @@
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E91" t="n">
@@ -4362,7 +4362,7 @@
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E92" t="n">
@@ -4405,7 +4405,7 @@
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E93" t="n">
@@ -4448,7 +4448,7 @@
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E94" t="n">
@@ -4491,7 +4491,7 @@
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E95" t="n">
@@ -4534,7 +4534,7 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E96" t="n">
@@ -4577,7 +4577,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E97" t="n">
@@ -4620,7 +4620,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E98" t="n">
@@ -4663,7 +4663,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E99" t="n">
@@ -4706,7 +4706,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E100" t="n">
@@ -4749,7 +4749,7 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E101" t="n">
@@ -4792,7 +4792,7 @@
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E102" t="n">
@@ -4835,7 +4835,7 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E103" t="n">
@@ -4878,7 +4878,7 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E104" t="n">
@@ -4921,7 +4921,7 @@
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E105" t="n">
@@ -4964,7 +4964,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E106" t="n">
@@ -5007,7 +5007,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E107" t="n">
@@ -5050,7 +5050,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E108" t="n">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E109" t="n">
@@ -5136,7 +5136,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E110" t="n">
@@ -5179,7 +5179,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E111" t="n">
@@ -5222,7 +5222,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E112" t="n">
@@ -5265,7 +5265,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E113" t="n">
@@ -5308,7 +5308,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E114" t="n">
@@ -5351,7 +5351,7 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E115" t="n">
@@ -5394,7 +5394,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E116" t="n">
@@ -5437,7 +5437,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E117" t="n">
@@ -5480,7 +5480,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E118" t="n">
@@ -5523,7 +5523,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E119" t="n">
@@ -5566,7 +5566,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E120" t="n">
@@ -5609,7 +5609,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E121" t="n">
@@ -5652,7 +5652,7 @@
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Consumer Discretionary</t>
+          <t>Consumer Cyclical</t>
         </is>
       </c>
       <c r="E122" t="n">

</xml_diff>